<commit_message>
Updates to structure and data files to support peaking calculations. Peaks now calculated based on ratio of peak seasonal demand by end use to average annual peak demand (we found a new data source to allow for this estimation). We no longer need the seasonal share of energy consutmpion so I've removed the folder structure and data files.
The results in early years are reasonable and I'm working on updating the data ensure the later years produce reasonable results (right now our peak demand is a bit too high).

I also reinstated RM because the peak demand numbers came more in line with actual demand, meaning the RM is back to serving a purpose (and not incorporated into the underying data).
</commit_message>
<xml_diff>
--- a/InputData/elec/RM/Reserve Margin.xlsx
+++ b/InputData/elec/RM/Reserve Margin.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\elec\RM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI - units progress\InputData\elec\RM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4A1AEC-17DD-45EC-BAEA-94DBCB9BD6B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="750" windowWidth="24750" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="22995" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>RM Reserve Margin</t>
   </si>
@@ -57,24 +56,12 @@
   </si>
   <si>
     <t>(dimensionless)</t>
-  </si>
-  <si>
-    <t>U.S. EPS 3.0.0 Note</t>
-  </si>
-  <si>
-    <t>In EPS 3.0.0, a new peaking calculation approach was adopted.  The new approach uses Equipment Load Factors (ELFs)</t>
-  </si>
-  <si>
-    <t>that may already account for some or all of the reserve margin that utilities consider.  We set the reservere margin to</t>
-  </si>
-  <si>
-    <t>zero, but we leave the data reference above in place in case we wish to use a non-zero reserve margin in the future.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -212,23 +199,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -264,23 +234,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -456,19 +409,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -476,64 +431,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="2">
         <v>2015</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -543,20 +478,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -669,117 +606,117 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="C2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="D2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="E2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="F2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="G2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="H2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="I2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="J2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="K2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="L2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="M2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="N2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="O2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="P2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="Q2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="R2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="S2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="T2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="U2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="V2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="W2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="X2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="Y2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="Z2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="AA2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="AB2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="AC2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="AD2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="AE2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="AF2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="AG2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="AH2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="AI2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="AJ2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
       <c r="AK2" s="3">
-        <v>0</v>
+        <v>0.14119999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>